<commit_message>
Using a load cell, but I kept the serial communication
</commit_message>
<xml_diff>
--- a/dados_do_paciente.xlsx
+++ b/dados_do_paciente.xlsx
@@ -450,13 +450,13 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>708</v>
+        <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>-7.5</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Using Threading and signals with PyQt5 and improving data acquisition. Still have stack overflow issues, but it's going in the right way.
</commit_message>
<xml_diff>
--- a/dados_do_paciente.xlsx
+++ b/dados_do_paciente.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -424,38 +424,36 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>Name</t>
+          <t>Position</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>Strength Peak</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>Development of Strength</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>Decline Rate</t>
+          <t>Value</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>John Doe</t>
-        </is>
+      <c r="A2" t="n">
+        <v>0</v>
       </c>
       <c r="B2" t="n">
         <v>0</v>
       </c>
-      <c r="C2" t="n">
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="n">
         <v>0</v>
       </c>
-      <c r="D2" t="n">
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
New model for threading. Arguments direct added to methods
</commit_message>
<xml_diff>
--- a/dados_do_paciente.xlsx
+++ b/dados_do_paciente.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -422,39 +422,113 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>Position</t>
-        </is>
+      <c r="A1" t="n">
+        <v>0</v>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>Value</t>
+          <t xml:space="preserve">668
+</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>0</v>
-      </c>
-      <c r="B2" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">671
+</t>
+        </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" t="n">
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">676
+</t>
+        </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>2</v>
-      </c>
-      <c r="B4" t="n">
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">682
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">688
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">692
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">697
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">715
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">732
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">752
+</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>